<commit_message>
Reunião 20 de junho
</commit_message>
<xml_diff>
--- a/BEPE FAPESP/Javier_Novembro.xlsx
+++ b/BEPE FAPESP/Javier_Novembro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c0f5011ef4481e6a/St_App/BEPE FAPESP/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="20" documentId="11_B0C7F1F9A47B6A229016DFA565F6DED0FD8F6E19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9D0FE731-D0E6-4922-A889-216A1F074B30}"/>
+  <xr:revisionPtr revIDLastSave="30" documentId="11_B0C7F1F9A47B6A229016DFA565F6DED0FD8F6E19" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A04BB3D5-915F-4C3B-BEE5-9EABA97163E9}"/>
   <bookViews>
     <workbookView xWindow="-15300" yWindow="-18120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1704,8 +1704,8 @@
   </sheetPr>
   <dimension ref="A1:AB103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="89" zoomScaleNormal="89" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1717,9 +1717,9 @@
     <col min="5" max="5" width="26.88671875" style="6" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="20.5546875" style="11" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="20.5546875" style="14" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.5546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.5546875" style="6" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.77734375" style="11" customWidth="1"/>
+    <col min="9" max="9" width="16.21875" style="6" customWidth="1"/>
+    <col min="10" max="10" width="9.88671875" style="12" customWidth="1"/>
     <col min="11" max="11" width="8.33203125" style="14" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="14.109375" style="6" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="19.88671875" style="6" bestFit="1" customWidth="1"/>
@@ -2823,19 +2823,19 @@
         <v>10.018799999999999</v>
       </c>
       <c r="E24" s="171">
-        <f t="shared" ref="E24:E33" si="1">D24-$I$34</f>
+        <f>D24-$I$34</f>
         <v>8.7717399999999994</v>
       </c>
       <c r="F24" s="74">
-        <f t="shared" ref="F24:F33" si="2">STDEV(B24:C24)</f>
+        <f>STDEV(B24:C24)</f>
         <v>0.62112259659426405</v>
       </c>
       <c r="G24" s="75">
-        <f t="shared" ref="G24:G33" si="3">E24/(150*$F$20/0.9)*100</f>
+        <f t="shared" ref="G24:G33" si="1">E24/(150*$F$20/0.9)*100</f>
         <v>7.9084057099924863</v>
       </c>
       <c r="H24" s="74">
-        <f t="shared" ref="H24:I30" si="4">H7*$I$18</f>
+        <f t="shared" ref="H24:I30" si="2">H7*$I$18</f>
         <v>0</v>
       </c>
       <c r="I24" s="82">
@@ -2854,27 +2854,27 @@
         <v>1.5384</v>
       </c>
       <c r="N24" s="77">
-        <f t="shared" ref="N24:N33" si="5">AVERAGE(L24:M24)</f>
+        <f t="shared" ref="N24:N33" si="3">AVERAGE(L24:M24)</f>
         <v>1.5636000000000001</v>
       </c>
       <c r="O24" s="171">
-        <f t="shared" ref="O24:O33" si="6">N24-$S$34</f>
+        <f t="shared" ref="O24:O33" si="4">N24-$S$34</f>
         <v>1.43469</v>
       </c>
       <c r="P24" s="78">
-        <f t="shared" ref="P24:P33" si="7">STDEV(L24:M24)</f>
+        <f t="shared" ref="P24:P33" si="5">STDEV(L24:M24)</f>
         <v>3.5638181771801995E-2</v>
       </c>
       <c r="Q24" s="110">
-        <f t="shared" ref="Q24:Q33" si="8">O24/(150*$O$20/0.88)*100</f>
+        <f t="shared" ref="Q24:Q33" si="6">O24/(150*$O$20/0.88)*100</f>
         <v>10.264448780487804</v>
       </c>
       <c r="R24" s="78">
-        <f t="shared" ref="R24:S30" si="9">R7*$I$18</f>
+        <f t="shared" ref="R24:S30" si="7">R7*$I$18</f>
         <v>0</v>
       </c>
       <c r="S24" s="123">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1.7999999999999999E-2</v>
       </c>
       <c r="T24" s="13"/>
@@ -2890,23 +2890,23 @@
         <v>0.36119999999999997</v>
       </c>
       <c r="X24" s="80">
-        <f t="shared" ref="X24:X33" si="10">AVERAGE(V24:W24)</f>
+        <f t="shared" ref="X24:X33" si="8">AVERAGE(V24:W24)</f>
         <v>0.38400000000000001</v>
       </c>
       <c r="Y24" s="171">
-        <f t="shared" ref="Y24:Y33" si="11">X24-$AB$34</f>
+        <f t="shared" ref="Y24:Y33" si="9">X24-$AB$34</f>
         <v>0.17485999999999999</v>
       </c>
       <c r="Z24" s="81">
-        <f t="shared" ref="Z24:Z33" si="12">STDEV(V24:W24)</f>
+        <f t="shared" ref="Z24:Z33" si="10">STDEV(V24:W24)</f>
         <v>3.224406922210659E-2</v>
       </c>
       <c r="AA24" s="81">
-        <f t="shared" ref="AA24:AB30" si="13">AA7*$I$18</f>
+        <f t="shared" ref="AA24:AB30" si="11">AA7*$I$18</f>
         <v>0</v>
       </c>
       <c r="AB24" s="83">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0.2412</v>
       </c>
     </row>
@@ -2915,11 +2915,11 @@
         <v>2</v>
       </c>
       <c r="B25" s="73">
-        <f t="shared" ref="B25:C30" si="14">B8*$J$18</f>
+        <f t="shared" ref="B25:C30" si="12">B8*$J$18</f>
         <v>15.576000000000001</v>
       </c>
       <c r="C25" s="73">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>13.644</v>
       </c>
       <c r="D25" s="73">
@@ -2927,23 +2927,23 @@
         <v>14.61</v>
       </c>
       <c r="E25" s="171">
+        <f t="shared" ref="E24:E33" si="13">D25-$I$34</f>
+        <v>13.36294</v>
+      </c>
+      <c r="F25" s="74">
+        <f t="shared" ref="F24:F33" si="14">STDEV(B25:C25)</f>
+        <v>1.36613030125241</v>
+      </c>
+      <c r="G25" s="75">
         <f t="shared" si="1"/>
-        <v>13.36294</v>
-      </c>
-      <c r="F25" s="74">
+        <v>12.047729526671674</v>
+      </c>
+      <c r="H25" s="74">
         <f t="shared" si="2"/>
-        <v>1.36613030125241</v>
-      </c>
-      <c r="G25" s="75">
-        <f t="shared" si="3"/>
-        <v>12.047729526671674</v>
-      </c>
-      <c r="H25" s="74">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I25" s="82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1.2155999999999998</v>
       </c>
       <c r="K25" s="170">
@@ -2958,27 +2958,27 @@
         <v>2.052</v>
       </c>
       <c r="N25" s="77">
+        <f t="shared" si="3"/>
+        <v>2.1360000000000001</v>
+      </c>
+      <c r="O25" s="171">
+        <f t="shared" si="4"/>
+        <v>2.0070900000000003</v>
+      </c>
+      <c r="P25" s="78">
         <f t="shared" si="5"/>
-        <v>2.1360000000000001</v>
-      </c>
-      <c r="O25" s="171">
+        <v>0.11879393923933977</v>
+      </c>
+      <c r="Q25" s="110">
         <f t="shared" si="6"/>
-        <v>2.0070900000000003</v>
-      </c>
-      <c r="P25" s="78">
+        <v>14.359668292682928</v>
+      </c>
+      <c r="R25" s="78">
         <f t="shared" si="7"/>
-        <v>0.11879393923933977</v>
-      </c>
-      <c r="Q25" s="110">
-        <f t="shared" si="8"/>
-        <v>14.359668292682928</v>
-      </c>
-      <c r="R25" s="78">
-        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="S25" s="123">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1.9199999999999998E-2</v>
       </c>
       <c r="T25" s="13"/>
@@ -2994,23 +2994,23 @@
         <v>0.56400000000000006</v>
       </c>
       <c r="X25" s="80">
+        <f t="shared" si="8"/>
+        <v>0.57600000000000007</v>
+      </c>
+      <c r="Y25" s="171">
+        <f t="shared" si="9"/>
+        <v>0.36686000000000007</v>
+      </c>
+      <c r="Z25" s="81">
         <f t="shared" si="10"/>
-        <v>0.57600000000000007</v>
-      </c>
-      <c r="Y25" s="171">
+        <v>1.6970562748477157E-2</v>
+      </c>
+      <c r="AA25" s="81">
         <f t="shared" si="11"/>
-        <v>0.36686000000000007</v>
-      </c>
-      <c r="Z25" s="81">
-        <f t="shared" si="12"/>
-        <v>1.6970562748477157E-2</v>
-      </c>
-      <c r="AA25" s="81">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AB25" s="83">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0.2316</v>
       </c>
     </row>
@@ -3019,11 +3019,11 @@
         <v>4</v>
       </c>
       <c r="B26" s="73">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>25.523999999999997</v>
       </c>
       <c r="C26" s="73">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>23.16</v>
       </c>
       <c r="D26" s="73">
@@ -3031,23 +3031,23 @@
         <v>24.341999999999999</v>
       </c>
       <c r="E26" s="171">
+        <f t="shared" si="13"/>
+        <v>23.094939999999998</v>
+      </c>
+      <c r="F26" s="74">
+        <f t="shared" si="14"/>
+        <v>1.6716004307249963</v>
+      </c>
+      <c r="G26" s="75">
         <f t="shared" si="1"/>
-        <v>23.094939999999998</v>
-      </c>
-      <c r="F26" s="74">
+        <v>20.821884297520658</v>
+      </c>
+      <c r="H26" s="74">
         <f t="shared" si="2"/>
-        <v>1.6716004307249963</v>
-      </c>
-      <c r="G26" s="75">
-        <f t="shared" si="3"/>
-        <v>20.821884297520658</v>
-      </c>
-      <c r="H26" s="74">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I26" s="82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1.2371999999999999</v>
       </c>
       <c r="K26" s="170">
@@ -3062,27 +3062,27 @@
         <v>2.9159999999999999</v>
       </c>
       <c r="N26" s="77">
+        <f t="shared" si="3"/>
+        <v>2.9580000000000002</v>
+      </c>
+      <c r="O26" s="171">
+        <f t="shared" si="4"/>
+        <v>2.8290900000000003</v>
+      </c>
+      <c r="P26" s="78">
         <f t="shared" si="5"/>
-        <v>2.9580000000000002</v>
-      </c>
-      <c r="O26" s="171">
+        <v>5.9396969619670045E-2</v>
+      </c>
+      <c r="Q26" s="110">
         <f t="shared" si="6"/>
-        <v>2.8290900000000003</v>
-      </c>
-      <c r="P26" s="78">
+        <v>20.240643902439025</v>
+      </c>
+      <c r="R26" s="78">
         <f t="shared" si="7"/>
-        <v>5.9396969619670045E-2</v>
-      </c>
-      <c r="Q26" s="110">
-        <f t="shared" si="8"/>
-        <v>20.240643902439025</v>
-      </c>
-      <c r="R26" s="78">
-        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="S26" s="123">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1.5599999999999999E-2</v>
       </c>
       <c r="T26" s="13"/>
@@ -3098,23 +3098,23 @@
         <v>0.85199999999999987</v>
       </c>
       <c r="X26" s="80">
+        <f t="shared" si="8"/>
+        <v>0.89999999999999991</v>
+      </c>
+      <c r="Y26" s="171">
+        <f t="shared" si="9"/>
+        <v>0.69085999999999992</v>
+      </c>
+      <c r="Z26" s="81">
         <f t="shared" si="10"/>
-        <v>0.89999999999999991</v>
-      </c>
-      <c r="Y26" s="171">
+        <v>6.7882250993908627E-2</v>
+      </c>
+      <c r="AA26" s="81">
         <f t="shared" si="11"/>
-        <v>0.69085999999999992</v>
-      </c>
-      <c r="Z26" s="81">
-        <f t="shared" si="12"/>
-        <v>6.7882250993908627E-2</v>
-      </c>
-      <c r="AA26" s="81">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AB26" s="83">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0.22919999999999999</v>
       </c>
     </row>
@@ -3123,11 +3123,11 @@
         <v>6</v>
       </c>
       <c r="B27" s="73">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>31.356000000000002</v>
       </c>
       <c r="C27" s="73">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>28.86</v>
       </c>
       <c r="D27" s="73">
@@ -3135,23 +3135,23 @@
         <v>30.108000000000001</v>
       </c>
       <c r="E27" s="171">
+        <f t="shared" si="13"/>
+        <v>28.860939999999999</v>
+      </c>
+      <c r="F27" s="74">
+        <f t="shared" si="14"/>
+        <v>1.7649385258416241</v>
+      </c>
+      <c r="G27" s="75">
         <f t="shared" si="1"/>
-        <v>28.860939999999999</v>
-      </c>
-      <c r="F27" s="74">
+        <v>26.020381667918858</v>
+      </c>
+      <c r="H27" s="74">
         <f t="shared" si="2"/>
-        <v>1.7649385258416241</v>
-      </c>
-      <c r="G27" s="75">
-        <f t="shared" si="3"/>
-        <v>26.020381667918858</v>
-      </c>
-      <c r="H27" s="74">
-        <f t="shared" si="4"/>
         <v>0.26639999999999997</v>
       </c>
       <c r="I27" s="82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1.2419999999999998</v>
       </c>
       <c r="K27" s="170">
@@ -3166,27 +3166,27 @@
         <v>3.2760000000000002</v>
       </c>
       <c r="N27" s="77">
+        <f t="shared" si="3"/>
+        <v>3.33</v>
+      </c>
+      <c r="O27" s="171">
+        <f t="shared" si="4"/>
+        <v>3.2010900000000002</v>
+      </c>
+      <c r="P27" s="78">
         <f t="shared" si="5"/>
-        <v>3.33</v>
-      </c>
-      <c r="O27" s="171">
+        <v>7.6367532368146571E-2</v>
+      </c>
+      <c r="Q27" s="110">
         <f t="shared" si="6"/>
-        <v>3.2010900000000002</v>
-      </c>
-      <c r="P27" s="78">
+        <v>22.90210731707317</v>
+      </c>
+      <c r="R27" s="78">
         <f t="shared" si="7"/>
-        <v>7.6367532368146571E-2</v>
-      </c>
-      <c r="Q27" s="110">
-        <f t="shared" si="8"/>
-        <v>22.90210731707317</v>
-      </c>
-      <c r="R27" s="78">
-        <f t="shared" si="9"/>
         <v>1.5599999999999999E-2</v>
       </c>
       <c r="S27" s="123">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1.5599999999999999E-2</v>
       </c>
       <c r="T27" s="13"/>
@@ -3202,23 +3202,23 @@
         <v>1.056</v>
       </c>
       <c r="X27" s="80">
+        <f t="shared" si="8"/>
+        <v>1.032</v>
+      </c>
+      <c r="Y27" s="171">
+        <f t="shared" si="9"/>
+        <v>0.82286000000000004</v>
+      </c>
+      <c r="Z27" s="81">
         <f t="shared" si="10"/>
-        <v>1.032</v>
-      </c>
-      <c r="Y27" s="171">
+        <v>3.3941125496954314E-2</v>
+      </c>
+      <c r="AA27" s="81">
         <f t="shared" si="11"/>
-        <v>0.82286000000000004</v>
-      </c>
-      <c r="Z27" s="81">
-        <f t="shared" si="12"/>
-        <v>3.3941125496954314E-2</v>
-      </c>
-      <c r="AA27" s="81">
-        <f t="shared" si="13"/>
         <v>1.5599999999999999E-2</v>
       </c>
       <c r="AB27" s="83">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0.22799999999999998</v>
       </c>
     </row>
@@ -3227,11 +3227,11 @@
         <v>8</v>
       </c>
       <c r="B28" s="73">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>34.811999999999998</v>
       </c>
       <c r="C28" s="73">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>33.875999999999998</v>
       </c>
       <c r="D28" s="73">
@@ -3239,23 +3239,23 @@
         <v>34.343999999999994</v>
       </c>
       <c r="E28" s="171">
+        <f t="shared" si="13"/>
+        <v>33.096939999999996</v>
+      </c>
+      <c r="F28" s="74">
+        <f t="shared" si="14"/>
+        <v>0.66185194719060847</v>
+      </c>
+      <c r="G28" s="75">
         <f t="shared" si="1"/>
-        <v>33.096939999999996</v>
-      </c>
-      <c r="F28" s="74">
+        <v>29.839465063861752</v>
+      </c>
+      <c r="H28" s="74">
         <f t="shared" si="2"/>
-        <v>0.66185194719060847</v>
-      </c>
-      <c r="G28" s="75">
-        <f t="shared" si="3"/>
-        <v>29.839465063861752</v>
-      </c>
-      <c r="H28" s="74">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I28" s="82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1.2539999999999998</v>
       </c>
       <c r="K28" s="170">
@@ -3270,27 +3270,27 @@
         <v>3.6479999999999997</v>
       </c>
       <c r="N28" s="77">
+        <f t="shared" si="3"/>
+        <v>3.63</v>
+      </c>
+      <c r="O28" s="171">
+        <f t="shared" si="4"/>
+        <v>3.50109</v>
+      </c>
+      <c r="P28" s="78">
         <f t="shared" si="5"/>
-        <v>3.63</v>
-      </c>
-      <c r="O28" s="171">
+        <v>2.5455844122715419E-2</v>
+      </c>
+      <c r="Q28" s="110">
         <f t="shared" si="6"/>
-        <v>3.50109</v>
-      </c>
-      <c r="P28" s="78">
+        <v>25.048448780487803</v>
+      </c>
+      <c r="R28" s="78">
         <f t="shared" si="7"/>
-        <v>2.5455844122715419E-2</v>
-      </c>
-      <c r="Q28" s="110">
-        <f t="shared" si="8"/>
-        <v>25.048448780487803</v>
-      </c>
-      <c r="R28" s="78">
-        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="S28" s="123">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1.6799999999999999E-2</v>
       </c>
       <c r="T28" s="13"/>
@@ -3306,23 +3306,23 @@
         <v>1.1640000000000001</v>
       </c>
       <c r="X28" s="80">
+        <f t="shared" si="8"/>
+        <v>1.1340000000000001</v>
+      </c>
+      <c r="Y28" s="171">
+        <f t="shared" si="9"/>
+        <v>0.92486000000000013</v>
+      </c>
+      <c r="Z28" s="81">
         <f t="shared" si="10"/>
-        <v>1.1340000000000001</v>
-      </c>
-      <c r="Y28" s="171">
+        <v>4.2426406871192889E-2</v>
+      </c>
+      <c r="AA28" s="81">
         <f t="shared" si="11"/>
-        <v>0.92486000000000013</v>
-      </c>
-      <c r="Z28" s="81">
-        <f t="shared" si="12"/>
-        <v>4.2426406871192889E-2</v>
-      </c>
-      <c r="AA28" s="81">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AB28" s="83">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0.2268</v>
       </c>
     </row>
@@ -3331,11 +3331,11 @@
         <v>12</v>
       </c>
       <c r="B29" s="73">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>38.688000000000002</v>
       </c>
       <c r="C29" s="73">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>38.352000000000004</v>
       </c>
       <c r="D29" s="73">
@@ -3343,23 +3343,23 @@
         <v>38.520000000000003</v>
       </c>
       <c r="E29" s="171">
+        <f t="shared" si="13"/>
+        <v>37.272940000000006</v>
+      </c>
+      <c r="F29" s="74">
+        <f t="shared" si="14"/>
+        <v>0.23758787847867893</v>
+      </c>
+      <c r="G29" s="75">
         <f t="shared" si="1"/>
-        <v>37.272940000000006</v>
-      </c>
-      <c r="F29" s="74">
+        <v>33.604453794139751</v>
+      </c>
+      <c r="H29" s="74">
         <f t="shared" si="2"/>
-        <v>0.23758787847867893</v>
-      </c>
-      <c r="G29" s="75">
-        <f t="shared" si="3"/>
-        <v>33.604453794139751</v>
-      </c>
-      <c r="H29" s="74">
-        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="I29" s="82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1.2647999999999999</v>
       </c>
       <c r="K29" s="170">
@@ -3374,27 +3374,27 @@
         <v>4.008</v>
       </c>
       <c r="N29" s="77">
+        <f t="shared" si="3"/>
+        <v>3.96</v>
+      </c>
+      <c r="O29" s="171">
+        <f t="shared" si="4"/>
+        <v>3.8310900000000001</v>
+      </c>
+      <c r="P29" s="78">
         <f t="shared" si="5"/>
-        <v>3.96</v>
-      </c>
-      <c r="O29" s="171">
+        <v>6.7882250993908627E-2</v>
+      </c>
+      <c r="Q29" s="110">
         <f t="shared" si="6"/>
-        <v>3.8310900000000001</v>
-      </c>
-      <c r="P29" s="78">
+        <v>27.409424390243903</v>
+      </c>
+      <c r="R29" s="78">
         <f t="shared" si="7"/>
-        <v>6.7882250993908627E-2</v>
-      </c>
-      <c r="Q29" s="110">
-        <f t="shared" si="8"/>
-        <v>27.409424390243903</v>
-      </c>
-      <c r="R29" s="78">
-        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="S29" s="123">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1.9199999999999998E-2</v>
       </c>
       <c r="T29" s="13"/>
@@ -3410,23 +3410,23 @@
         <v>1.296</v>
       </c>
       <c r="X29" s="80">
+        <f t="shared" si="8"/>
+        <v>1.26</v>
+      </c>
+      <c r="Y29" s="171">
+        <f t="shared" si="9"/>
+        <v>1.0508599999999999</v>
+      </c>
+      <c r="Z29" s="81">
         <f t="shared" si="10"/>
-        <v>1.26</v>
-      </c>
-      <c r="Y29" s="171">
+        <v>5.0911688245431463E-2</v>
+      </c>
+      <c r="AA29" s="81">
         <f t="shared" si="11"/>
-        <v>1.0508599999999999</v>
-      </c>
-      <c r="Z29" s="81">
-        <f t="shared" si="12"/>
-        <v>5.0911688245431463E-2</v>
-      </c>
-      <c r="AA29" s="81">
-        <f t="shared" si="13"/>
         <v>0</v>
       </c>
       <c r="AB29" s="83">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0.22559999999999999</v>
       </c>
     </row>
@@ -3435,11 +3435,11 @@
         <v>24</v>
       </c>
       <c r="B30" s="73">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>47.027999999999999</v>
       </c>
       <c r="C30" s="73">
-        <f t="shared" si="14"/>
+        <f t="shared" si="12"/>
         <v>46.176000000000002</v>
       </c>
       <c r="D30" s="73">
@@ -3447,23 +3447,23 @@
         <v>46.602000000000004</v>
       </c>
       <c r="E30" s="171">
+        <f t="shared" si="13"/>
+        <v>45.354940000000006</v>
+      </c>
+      <c r="F30" s="74">
+        <f t="shared" si="14"/>
+        <v>0.60245497757093613</v>
+      </c>
+      <c r="G30" s="75">
         <f t="shared" si="1"/>
-        <v>45.354940000000006</v>
-      </c>
-      <c r="F30" s="74">
+        <v>40.89100525920361</v>
+      </c>
+      <c r="H30" s="74">
         <f t="shared" si="2"/>
-        <v>0.60245497757093613</v>
-      </c>
-      <c r="G30" s="75">
-        <f t="shared" si="3"/>
-        <v>40.89100525920361</v>
-      </c>
-      <c r="H30" s="74">
-        <f t="shared" si="4"/>
         <v>0.108</v>
       </c>
       <c r="I30" s="82">
-        <f t="shared" si="4"/>
+        <f t="shared" si="2"/>
         <v>1.2816000000000001</v>
       </c>
       <c r="K30" s="170">
@@ -3478,27 +3478,27 @@
         <v>4.5960000000000001</v>
       </c>
       <c r="N30" s="77">
+        <f t="shared" si="3"/>
+        <v>4.5839999999999996</v>
+      </c>
+      <c r="O30" s="171">
+        <f t="shared" si="4"/>
+        <v>4.4550899999999993</v>
+      </c>
+      <c r="P30" s="78">
         <f t="shared" si="5"/>
-        <v>4.5839999999999996</v>
-      </c>
-      <c r="O30" s="171">
+        <v>1.6970562748477157E-2</v>
+      </c>
+      <c r="Q30" s="110">
         <f t="shared" si="6"/>
-        <v>4.4550899999999993</v>
-      </c>
-      <c r="P30" s="78">
+        <v>31.873814634146335</v>
+      </c>
+      <c r="R30" s="78">
         <f t="shared" si="7"/>
-        <v>1.6970562748477157E-2</v>
-      </c>
-      <c r="Q30" s="110">
-        <f t="shared" si="8"/>
-        <v>31.873814634146335</v>
-      </c>
-      <c r="R30" s="78">
-        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="S30" s="123">
-        <f t="shared" si="9"/>
+        <f t="shared" si="7"/>
         <v>1.6799999999999999E-2</v>
       </c>
       <c r="T30" s="13"/>
@@ -3514,23 +3514,23 @@
         <v>1.6320000000000001</v>
       </c>
       <c r="X30" s="80">
+        <f t="shared" si="8"/>
+        <v>1.62</v>
+      </c>
+      <c r="Y30" s="171">
+        <f t="shared" si="9"/>
+        <v>1.41086</v>
+      </c>
+      <c r="Z30" s="81">
         <f t="shared" si="10"/>
-        <v>1.62</v>
-      </c>
-      <c r="Y30" s="171">
+        <v>1.6970562748477157E-2</v>
+      </c>
+      <c r="AA30" s="81">
         <f t="shared" si="11"/>
-        <v>1.41086</v>
-      </c>
-      <c r="Z30" s="81">
-        <f t="shared" si="12"/>
-        <v>1.6970562748477157E-2</v>
-      </c>
-      <c r="AA30" s="81">
-        <f t="shared" si="13"/>
         <v>1.0799999999999999E-2</v>
       </c>
       <c r="AB30" s="83">
-        <f t="shared" si="13"/>
+        <f t="shared" si="11"/>
         <v>0.216</v>
       </c>
     </row>
@@ -3551,15 +3551,15 @@
         <v>54.808000000000007</v>
       </c>
       <c r="E31" s="171">
+        <f t="shared" si="13"/>
+        <v>53.560940000000009</v>
+      </c>
+      <c r="F31" s="74">
+        <f t="shared" si="14"/>
+        <v>2.5243712088359747</v>
+      </c>
+      <c r="G31" s="75">
         <f t="shared" si="1"/>
-        <v>53.560940000000009</v>
-      </c>
-      <c r="F31" s="74">
-        <f t="shared" si="2"/>
-        <v>2.5243712088359747</v>
-      </c>
-      <c r="G31" s="75">
-        <f t="shared" si="3"/>
         <v>48.28935236664163</v>
       </c>
       <c r="H31" s="74">
@@ -3582,19 +3582,19 @@
         <v>8.4320000000000004</v>
       </c>
       <c r="N31" s="77">
+        <f t="shared" si="3"/>
+        <v>7.8369999999999997</v>
+      </c>
+      <c r="O31" s="171">
+        <f t="shared" si="4"/>
+        <v>7.7080899999999994</v>
+      </c>
+      <c r="P31" s="78">
         <f t="shared" si="5"/>
-        <v>7.8369999999999997</v>
-      </c>
-      <c r="O31" s="171">
+        <v>0.84145706961199185</v>
+      </c>
+      <c r="Q31" s="110">
         <f t="shared" si="6"/>
-        <v>7.7080899999999994</v>
-      </c>
-      <c r="P31" s="78">
-        <f t="shared" si="7"/>
-        <v>0.84145706961199185</v>
-      </c>
-      <c r="Q31" s="110">
-        <f t="shared" si="8"/>
         <v>55.147310569105677</v>
       </c>
       <c r="R31" s="78">
@@ -3618,15 +3618,15 @@
         <v>1.377</v>
       </c>
       <c r="X31" s="80">
+        <f t="shared" si="8"/>
+        <v>1.2919999999999998</v>
+      </c>
+      <c r="Y31" s="171">
+        <f t="shared" si="9"/>
+        <v>1.0828599999999997</v>
+      </c>
+      <c r="Z31" s="81">
         <f t="shared" si="10"/>
-        <v>1.2919999999999998</v>
-      </c>
-      <c r="Y31" s="171">
-        <f t="shared" si="11"/>
-        <v>1.0828599999999997</v>
-      </c>
-      <c r="Z31" s="81">
-        <f t="shared" si="12"/>
         <v>0.12020815280171318</v>
       </c>
       <c r="AA31" s="81">
@@ -3655,15 +3655,15 @@
         <v>57.153999999999996</v>
       </c>
       <c r="E32" s="171">
+        <f t="shared" si="13"/>
+        <v>55.906939999999999</v>
+      </c>
+      <c r="F32" s="74">
+        <f t="shared" si="14"/>
+        <v>2.3079965337928932</v>
+      </c>
+      <c r="G32" s="75">
         <f t="shared" si="1"/>
-        <v>55.906939999999999</v>
-      </c>
-      <c r="F32" s="74">
-        <f t="shared" si="2"/>
-        <v>2.3079965337928932</v>
-      </c>
-      <c r="G32" s="75">
-        <f t="shared" si="3"/>
         <v>50.404453794139734</v>
       </c>
       <c r="H32" s="74">
@@ -3686,19 +3686,19 @@
         <v>8.2110000000000003</v>
       </c>
       <c r="N32" s="77">
+        <f t="shared" si="3"/>
+        <v>8.0665000000000013</v>
+      </c>
+      <c r="O32" s="171">
+        <f t="shared" si="4"/>
+        <v>7.937590000000001</v>
+      </c>
+      <c r="P32" s="78">
         <f t="shared" si="5"/>
-        <v>8.0665000000000013</v>
-      </c>
-      <c r="O32" s="171">
+        <v>0.20435385976291204</v>
+      </c>
+      <c r="Q32" s="110">
         <f t="shared" si="6"/>
-        <v>7.937590000000001</v>
-      </c>
-      <c r="P32" s="78">
-        <f t="shared" si="7"/>
-        <v>0.20435385976291204</v>
-      </c>
-      <c r="Q32" s="110">
-        <f t="shared" si="8"/>
         <v>56.789261788617885</v>
       </c>
       <c r="R32" s="78">
@@ -3722,15 +3722,15 @@
         <v>1.1220000000000001</v>
       </c>
       <c r="X32" s="80">
+        <f t="shared" si="8"/>
+        <v>1.1560000000000001</v>
+      </c>
+      <c r="Y32" s="171">
+        <f t="shared" si="9"/>
+        <v>0.94686000000000015</v>
+      </c>
+      <c r="Z32" s="81">
         <f t="shared" si="10"/>
-        <v>1.1560000000000001</v>
-      </c>
-      <c r="Y32" s="171">
-        <f t="shared" si="11"/>
-        <v>0.94686000000000015</v>
-      </c>
-      <c r="Z32" s="81">
-        <f t="shared" si="12"/>
         <v>4.8083261120685276E-2</v>
       </c>
       <c r="AA32" s="81">
@@ -3759,15 +3759,15 @@
         <v>59.16</v>
       </c>
       <c r="E33" s="171">
+        <f t="shared" si="13"/>
+        <v>57.912939999999999</v>
+      </c>
+      <c r="F33" s="74">
+        <f t="shared" si="14"/>
+        <v>1.9473720753877504</v>
+      </c>
+      <c r="G33" s="75">
         <f t="shared" si="1"/>
-        <v>57.912939999999999</v>
-      </c>
-      <c r="F33" s="74">
-        <f t="shared" si="2"/>
-        <v>1.9473720753877504</v>
-      </c>
-      <c r="G33" s="75">
-        <f t="shared" si="3"/>
         <v>52.213018782870023</v>
       </c>
       <c r="H33" s="86">
@@ -3790,19 +3790,19 @@
         <v>8.6020000000000003</v>
       </c>
       <c r="N33" s="77">
+        <f t="shared" si="3"/>
+        <v>8.4915000000000003</v>
+      </c>
+      <c r="O33" s="171">
+        <f t="shared" si="4"/>
+        <v>8.3625900000000009</v>
+      </c>
+      <c r="P33" s="78">
         <f t="shared" si="5"/>
-        <v>8.4915000000000003</v>
-      </c>
-      <c r="O33" s="171">
+        <v>0.15627059864222706</v>
+      </c>
+      <c r="Q33" s="110">
         <f t="shared" si="6"/>
-        <v>8.3625900000000009</v>
-      </c>
-      <c r="P33" s="78">
-        <f t="shared" si="7"/>
-        <v>0.15627059864222706</v>
-      </c>
-      <c r="Q33" s="110">
-        <f t="shared" si="8"/>
         <v>59.829912195121949</v>
       </c>
       <c r="R33" s="90">
@@ -3826,15 +3826,15 @@
         <v>1.105</v>
       </c>
       <c r="X33" s="80">
+        <f t="shared" si="8"/>
+        <v>1.139</v>
+      </c>
+      <c r="Y33" s="171">
+        <f t="shared" si="9"/>
+        <v>0.92986000000000002</v>
+      </c>
+      <c r="Z33" s="81">
         <f t="shared" si="10"/>
-        <v>1.139</v>
-      </c>
-      <c r="Y33" s="171">
-        <f t="shared" si="11"/>
-        <v>0.92986000000000002</v>
-      </c>
-      <c r="Z33" s="81">
-        <f t="shared" si="12"/>
         <v>4.8083261120685276E-2</v>
       </c>
       <c r="AA33" s="93">
@@ -4140,7 +4140,7 @@
   </sheetPr>
   <dimension ref="A1:AB135"/>
   <sheetViews>
-    <sheetView topLeftCell="F10" workbookViewId="0">
+    <sheetView topLeftCell="A8" workbookViewId="0">
       <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
@@ -6751,7 +6751,9 @@
   </sheetPr>
   <dimension ref="A1:AB70"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:AA1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -8795,7 +8797,9 @@
   </sheetPr>
   <dimension ref="A1:AB72"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:AA1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -10862,12 +10866,14 @@
   </sheetPr>
   <dimension ref="A1:AB36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.5546875" style="12" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="12.109375" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.5546875" style="6" customWidth="1"/>
     <col min="3" max="3" width="11.33203125" style="50" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.33203125" style="131" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.6640625" style="6" bestFit="1" customWidth="1"/>
@@ -14377,7 +14383,9 @@
   </sheetPr>
   <dimension ref="A1:AB36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:AA1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>